<commit_message>
Move DC surplus heat
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_SRV_DC_ExcessHeat.xlsx
+++ b/SubRES_TMPL/SubRES_SRV_DC_ExcessHeat.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8847439-841E-458F-9A48-3CC38381B370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A48014D-F089-40DF-9FDA-681C19B19723}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="16" r:id="rId1"/>
@@ -2528,25 +2528,25 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="21.73046875" style="120" customWidth="1"/>
-    <col min="5" max="6" width="14.1328125" style="120" customWidth="1"/>
-    <col min="7" max="7" width="12.1328125" style="120" customWidth="1"/>
-    <col min="8" max="10" width="8.1328125" style="120" customWidth="1"/>
-    <col min="11" max="11" width="9.73046875" style="120" customWidth="1"/>
-    <col min="12" max="12" width="8.1328125" style="120" customWidth="1"/>
+    <col min="1" max="4" width="21.7109375" style="120" customWidth="1"/>
+    <col min="5" max="6" width="14.140625" style="120" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="120" customWidth="1"/>
+    <col min="8" max="10" width="8.140625" style="120" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" style="120" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" style="120" customWidth="1"/>
     <col min="13" max="13" width="10" style="120" customWidth="1"/>
-    <col min="14" max="14" width="11.3984375" style="120" customWidth="1"/>
-    <col min="15" max="15" width="13.3984375" style="120" customWidth="1"/>
-    <col min="16" max="16384" width="8.86328125" style="120"/>
+    <col min="14" max="14" width="11.42578125" style="120" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" style="120" customWidth="1"/>
+    <col min="16" max="16384" width="8.85546875" style="120"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="118"/>
       <c r="B1" s="118"/>
       <c r="C1" s="118"/>
@@ -2574,7 +2574,7 @@
       <c r="Y1" s="119"/>
       <c r="Z1" s="119"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="118"/>
       <c r="B2" s="118"/>
       <c r="C2" s="118"/>
@@ -2602,7 +2602,7 @@
       <c r="Y2" s="119"/>
       <c r="Z2" s="119"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="118"/>
       <c r="B3" s="118"/>
       <c r="C3" s="118"/>
@@ -2630,7 +2630,7 @@
       <c r="Y3" s="119"/>
       <c r="Z3" s="119"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="118"/>
       <c r="B4" s="118"/>
       <c r="C4" s="118"/>
@@ -2658,7 +2658,7 @@
       <c r="Y4" s="119"/>
       <c r="Z4" s="119"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="118"/>
       <c r="B5" s="118"/>
       <c r="C5" s="118"/>
@@ -2686,7 +2686,7 @@
       <c r="Y5" s="119"/>
       <c r="Z5" s="119"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="118"/>
       <c r="B6" s="118"/>
       <c r="C6" s="118"/>
@@ -2714,7 +2714,7 @@
       <c r="Y6" s="119"/>
       <c r="Z6" s="119"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="118"/>
       <c r="B7" s="118"/>
       <c r="C7" s="118"/>
@@ -2742,7 +2742,7 @@
       <c r="Y7" s="119"/>
       <c r="Z7" s="119"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="118"/>
       <c r="B8" s="118"/>
       <c r="C8" s="118"/>
@@ -2770,7 +2770,7 @@
       <c r="Y8" s="119"/>
       <c r="Z8" s="119"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="118"/>
       <c r="B9" s="118"/>
       <c r="C9" s="118"/>
@@ -2798,7 +2798,7 @@
       <c r="Y9" s="119"/>
       <c r="Z9" s="119"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="118"/>
       <c r="B10" s="118"/>
       <c r="C10" s="118"/>
@@ -2826,7 +2826,7 @@
       <c r="Y10" s="119"/>
       <c r="Z10" s="119"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="118"/>
       <c r="B11" s="118"/>
       <c r="C11" s="118"/>
@@ -2854,7 +2854,7 @@
       <c r="Y11" s="119"/>
       <c r="Z11" s="119"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="118"/>
       <c r="B12" s="118"/>
       <c r="C12" s="118"/>
@@ -2882,7 +2882,7 @@
       <c r="Y12" s="119"/>
       <c r="Z12" s="119"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="118"/>
       <c r="B13" s="118"/>
       <c r="C13" s="118"/>
@@ -2910,7 +2910,7 @@
       <c r="Y13" s="119"/>
       <c r="Z13" s="119"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="118"/>
       <c r="B14" s="118"/>
       <c r="C14" s="118"/>
@@ -2938,7 +2938,7 @@
       <c r="Y14" s="119"/>
       <c r="Z14" s="119"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="118"/>
       <c r="B15" s="118"/>
       <c r="C15" s="118"/>
@@ -2966,7 +2966,7 @@
       <c r="Y15" s="119"/>
       <c r="Z15" s="119"/>
     </row>
-    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="135" t="s">
         <v>264</v>
       </c>
@@ -2996,7 +2996,7 @@
       <c r="Y16" s="119"/>
       <c r="Z16" s="119"/>
     </row>
-    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="123"/>
       <c r="B17" s="123"/>
       <c r="C17" s="123"/>
@@ -3024,7 +3024,7 @@
       <c r="Y17" s="119"/>
       <c r="Z17" s="119"/>
     </row>
-    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="123"/>
       <c r="B18" s="123"/>
       <c r="C18" s="123"/>
@@ -3052,7 +3052,7 @@
       <c r="Y18" s="119"/>
       <c r="Z18" s="119"/>
     </row>
-    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="126" t="s">
         <v>265</v>
       </c>
@@ -3084,7 +3084,7 @@
       <c r="Y19" s="119"/>
       <c r="Z19" s="119"/>
     </row>
-    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="126" t="s">
         <v>266</v>
       </c>
@@ -3116,7 +3116,7 @@
       <c r="Y20" s="119"/>
       <c r="Z20" s="119"/>
     </row>
-    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="126" t="s">
         <v>267</v>
       </c>
@@ -3148,7 +3148,7 @@
       <c r="Y21" s="119"/>
       <c r="Z21" s="119"/>
     </row>
-    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="126"/>
       <c r="B22" s="129"/>
       <c r="C22" s="129"/>
@@ -3176,7 +3176,7 @@
       <c r="Y22" s="119"/>
       <c r="Z22" s="119"/>
     </row>
-    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="126" t="s">
         <v>268</v>
       </c>
@@ -3208,7 +3208,7 @@
       <c r="Y23" s="119"/>
       <c r="Z23" s="119"/>
     </row>
-    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="126"/>
       <c r="B24" s="129"/>
       <c r="C24" s="129"/>
@@ -3236,7 +3236,7 @@
       <c r="Y24" s="119"/>
       <c r="Z24" s="119"/>
     </row>
-    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="126"/>
       <c r="B25" s="129"/>
       <c r="C25" s="129"/>
@@ -3264,7 +3264,7 @@
       <c r="Y25" s="119"/>
       <c r="Z25" s="119"/>
     </row>
-    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="126" t="s">
         <v>270</v>
       </c>
@@ -3296,7 +3296,7 @@
       <c r="Y26" s="119"/>
       <c r="Z26" s="119"/>
     </row>
-    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="126"/>
       <c r="B27" s="129"/>
       <c r="C27" s="129"/>
@@ -3324,7 +3324,7 @@
       <c r="Y27" s="119"/>
       <c r="Z27" s="119"/>
     </row>
-    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="126"/>
       <c r="B28" s="129"/>
       <c r="C28" s="129"/>
@@ -3352,7 +3352,7 @@
       <c r="Y28" s="119"/>
       <c r="Z28" s="119"/>
     </row>
-    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="126" t="s">
         <v>271</v>
       </c>
@@ -3384,7 +3384,7 @@
       <c r="Y29" s="119"/>
       <c r="Z29" s="119"/>
     </row>
-    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="126" t="s">
         <v>272</v>
       </c>
@@ -3416,7 +3416,7 @@
       <c r="Y30" s="119"/>
       <c r="Z30" s="119"/>
     </row>
-    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="126" t="s">
         <v>274</v>
       </c>
@@ -3448,7 +3448,7 @@
       <c r="Y31" s="119"/>
       <c r="Z31" s="119"/>
     </row>
-    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="132"/>
       <c r="B32" s="133" t="s">
         <v>276</v>
@@ -3478,7 +3478,7 @@
       <c r="Y32" s="119"/>
       <c r="Z32" s="119"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="118"/>
       <c r="B33" s="118"/>
       <c r="C33" s="118"/>
@@ -3506,7 +3506,7 @@
       <c r="Y33" s="119"/>
       <c r="Z33" s="119"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="118"/>
       <c r="B34" s="118"/>
       <c r="C34" s="118"/>
@@ -3534,7 +3534,7 @@
       <c r="Y34" s="119"/>
       <c r="Z34" s="119"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="118"/>
       <c r="B35" s="118"/>
       <c r="C35" s="118"/>
@@ -3562,7 +3562,7 @@
       <c r="Y35" s="119"/>
       <c r="Z35" s="119"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="118"/>
       <c r="B36" s="118"/>
       <c r="C36" s="118"/>
@@ -3590,7 +3590,7 @@
       <c r="Y36" s="119"/>
       <c r="Z36" s="119"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="118"/>
       <c r="B37" s="118"/>
       <c r="C37" s="118"/>
@@ -3618,7 +3618,7 @@
       <c r="Y37" s="119"/>
       <c r="Z37" s="119"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="118"/>
       <c r="B38" s="118"/>
       <c r="C38" s="118"/>
@@ -3646,7 +3646,7 @@
       <c r="Y38" s="119"/>
       <c r="Z38" s="119"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="118"/>
       <c r="B39" s="118"/>
       <c r="C39" s="118"/>
@@ -3674,7 +3674,7 @@
       <c r="Y39" s="119"/>
       <c r="Z39" s="119"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="118"/>
       <c r="B40" s="118"/>
       <c r="C40" s="118"/>
@@ -3702,7 +3702,7 @@
       <c r="Y40" s="119"/>
       <c r="Z40" s="119"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="118"/>
       <c r="B41" s="118"/>
       <c r="C41" s="118"/>
@@ -3730,7 +3730,7 @@
       <c r="Y41" s="119"/>
       <c r="Z41" s="119"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="118"/>
       <c r="B42" s="118"/>
       <c r="C42" s="118"/>
@@ -3758,7 +3758,7 @@
       <c r="Y42" s="119"/>
       <c r="Z42" s="119"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="119"/>
       <c r="B43" s="119"/>
       <c r="C43" s="119"/>
@@ -3786,7 +3786,7 @@
       <c r="Y43" s="119"/>
       <c r="Z43" s="119"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="119"/>
       <c r="B44" s="119"/>
       <c r="C44" s="119"/>
@@ -3814,7 +3814,7 @@
       <c r="Y44" s="119"/>
       <c r="Z44" s="119"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="119"/>
       <c r="B45" s="119"/>
       <c r="C45" s="119"/>
@@ -3842,7 +3842,7 @@
       <c r="Y45" s="119"/>
       <c r="Z45" s="119"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="119"/>
       <c r="B46" s="119"/>
       <c r="C46" s="119"/>
@@ -3870,7 +3870,7 @@
       <c r="Y46" s="119"/>
       <c r="Z46" s="119"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="119"/>
       <c r="B47" s="119"/>
       <c r="C47" s="119"/>
@@ -3898,7 +3898,7 @@
       <c r="Y47" s="119"/>
       <c r="Z47" s="119"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="119"/>
       <c r="B48" s="119"/>
       <c r="C48" s="119"/>
@@ -3926,7 +3926,7 @@
       <c r="Y48" s="119"/>
       <c r="Z48" s="119"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" s="119"/>
       <c r="B49" s="119"/>
       <c r="C49" s="119"/>
@@ -3954,7 +3954,7 @@
       <c r="Y49" s="119"/>
       <c r="Z49" s="119"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" s="119"/>
       <c r="B50" s="119"/>
       <c r="C50" s="119"/>
@@ -3982,7 +3982,7 @@
       <c r="Y50" s="119"/>
       <c r="Z50" s="119"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="119"/>
       <c r="B51" s="119"/>
       <c r="C51" s="119"/>
@@ -4010,7 +4010,7 @@
       <c r="Y51" s="119"/>
       <c r="Z51" s="119"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" s="119"/>
       <c r="B52" s="119"/>
       <c r="C52" s="119"/>
@@ -4038,7 +4038,7 @@
       <c r="Y52" s="119"/>
       <c r="Z52" s="119"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="119"/>
       <c r="B53" s="119"/>
       <c r="C53" s="119"/>
@@ -4066,7 +4066,7 @@
       <c r="Y53" s="119"/>
       <c r="Z53" s="119"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" s="119"/>
       <c r="B54" s="119"/>
       <c r="C54" s="119"/>
@@ -4094,7 +4094,7 @@
       <c r="Y54" s="119"/>
       <c r="Z54" s="119"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="119"/>
       <c r="B55" s="119"/>
       <c r="C55" s="119"/>
@@ -4122,7 +4122,7 @@
       <c r="Y55" s="119"/>
       <c r="Z55" s="119"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" s="119"/>
       <c r="B56" s="119"/>
       <c r="C56" s="119"/>
@@ -4150,7 +4150,7 @@
       <c r="Y56" s="119"/>
       <c r="Z56" s="119"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" s="119"/>
       <c r="B57" s="119"/>
       <c r="C57" s="119"/>
@@ -4178,7 +4178,7 @@
       <c r="Y57" s="119"/>
       <c r="Z57" s="119"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" s="119"/>
       <c r="B58" s="119"/>
       <c r="C58" s="119"/>
@@ -4206,7 +4206,7 @@
       <c r="Y58" s="119"/>
       <c r="Z58" s="119"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" s="119"/>
       <c r="B59" s="119"/>
       <c r="C59" s="119"/>
@@ -4234,7 +4234,7 @@
       <c r="Y59" s="119"/>
       <c r="Z59" s="119"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="119"/>
       <c r="B60" s="119"/>
       <c r="C60" s="119"/>
@@ -4262,7 +4262,7 @@
       <c r="Y60" s="119"/>
       <c r="Z60" s="119"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" s="119"/>
       <c r="B61" s="119"/>
       <c r="C61" s="119"/>
@@ -4290,7 +4290,7 @@
       <c r="Y61" s="119"/>
       <c r="Z61" s="119"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="119"/>
       <c r="B62" s="119"/>
       <c r="C62" s="119"/>
@@ -4318,7 +4318,7 @@
       <c r="Y62" s="119"/>
       <c r="Z62" s="119"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="119"/>
       <c r="B63" s="119"/>
       <c r="C63" s="119"/>
@@ -4346,7 +4346,7 @@
       <c r="Y63" s="119"/>
       <c r="Z63" s="119"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" s="119"/>
       <c r="B64" s="119"/>
       <c r="C64" s="119"/>
@@ -4374,7 +4374,7 @@
       <c r="Y64" s="119"/>
       <c r="Z64" s="119"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" s="119"/>
       <c r="B65" s="119"/>
       <c r="C65" s="119"/>
@@ -4402,7 +4402,7 @@
       <c r="Y65" s="119"/>
       <c r="Z65" s="119"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" s="119"/>
       <c r="B66" s="119"/>
       <c r="C66" s="119"/>
@@ -4430,7 +4430,7 @@
       <c r="Y66" s="119"/>
       <c r="Z66" s="119"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" s="119"/>
       <c r="B67" s="119"/>
       <c r="C67" s="119"/>
@@ -4458,7 +4458,7 @@
       <c r="Y67" s="119"/>
       <c r="Z67" s="119"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A68" s="119"/>
       <c r="B68" s="119"/>
       <c r="C68" s="119"/>
@@ -4486,7 +4486,7 @@
       <c r="Y68" s="119"/>
       <c r="Z68" s="119"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A69" s="119"/>
       <c r="B69" s="119"/>
       <c r="C69" s="119"/>
@@ -4514,7 +4514,7 @@
       <c r="Y69" s="119"/>
       <c r="Z69" s="119"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A70" s="119"/>
       <c r="B70" s="119"/>
       <c r="C70" s="119"/>
@@ -4542,7 +4542,7 @@
       <c r="Y70" s="119"/>
       <c r="Z70" s="119"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A71" s="119"/>
       <c r="B71" s="119"/>
       <c r="C71" s="119"/>
@@ -4570,7 +4570,7 @@
       <c r="Y71" s="119"/>
       <c r="Z71" s="119"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A72" s="119"/>
       <c r="B72" s="119"/>
       <c r="C72" s="119"/>
@@ -4598,7 +4598,7 @@
       <c r="Y72" s="119"/>
       <c r="Z72" s="119"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A73" s="119"/>
       <c r="B73" s="119"/>
       <c r="C73" s="119"/>
@@ -4626,7 +4626,7 @@
       <c r="Y73" s="119"/>
       <c r="Z73" s="119"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A74" s="119"/>
       <c r="B74" s="119"/>
       <c r="C74" s="119"/>
@@ -4654,7 +4654,7 @@
       <c r="Y74" s="119"/>
       <c r="Z74" s="119"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A75" s="119"/>
       <c r="B75" s="119"/>
       <c r="C75" s="119"/>
@@ -4682,7 +4682,7 @@
       <c r="Y75" s="119"/>
       <c r="Z75" s="119"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A76" s="119"/>
       <c r="B76" s="119"/>
       <c r="C76" s="119"/>
@@ -4710,7 +4710,7 @@
       <c r="Y76" s="119"/>
       <c r="Z76" s="119"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A77" s="119"/>
       <c r="B77" s="119"/>
       <c r="C77" s="119"/>
@@ -4738,7 +4738,7 @@
       <c r="Y77" s="119"/>
       <c r="Z77" s="119"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A78" s="119"/>
       <c r="B78" s="119"/>
       <c r="C78" s="119"/>
@@ -4766,7 +4766,7 @@
       <c r="Y78" s="119"/>
       <c r="Z78" s="119"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A79" s="119"/>
       <c r="B79" s="119"/>
       <c r="C79" s="119"/>
@@ -4794,7 +4794,7 @@
       <c r="Y79" s="119"/>
       <c r="Z79" s="119"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A80" s="119"/>
       <c r="B80" s="119"/>
       <c r="C80" s="119"/>
@@ -4822,7 +4822,7 @@
       <c r="Y80" s="119"/>
       <c r="Z80" s="119"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A81" s="119"/>
       <c r="B81" s="119"/>
       <c r="C81" s="119"/>
@@ -4850,7 +4850,7 @@
       <c r="Y81" s="119"/>
       <c r="Z81" s="119"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A82" s="119"/>
       <c r="B82" s="119"/>
       <c r="C82" s="119"/>
@@ -4878,7 +4878,7 @@
       <c r="Y82" s="119"/>
       <c r="Z82" s="119"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A83" s="119"/>
       <c r="B83" s="119"/>
       <c r="C83" s="119"/>
@@ -4906,7 +4906,7 @@
       <c r="Y83" s="119"/>
       <c r="Z83" s="119"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A84" s="119"/>
       <c r="B84" s="119"/>
       <c r="C84" s="119"/>
@@ -4934,7 +4934,7 @@
       <c r="Y84" s="119"/>
       <c r="Z84" s="119"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A85" s="119"/>
       <c r="B85" s="119"/>
       <c r="C85" s="119"/>
@@ -4962,7 +4962,7 @@
       <c r="Y85" s="119"/>
       <c r="Z85" s="119"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A86" s="119"/>
       <c r="B86" s="119"/>
       <c r="C86" s="119"/>
@@ -4990,7 +4990,7 @@
       <c r="Y86" s="119"/>
       <c r="Z86" s="119"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A87" s="119"/>
       <c r="B87" s="119"/>
       <c r="C87" s="119"/>
@@ -5018,7 +5018,7 @@
       <c r="Y87" s="119"/>
       <c r="Z87" s="119"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A88" s="119"/>
       <c r="B88" s="119"/>
       <c r="C88" s="119"/>
@@ -5046,7 +5046,7 @@
       <c r="Y88" s="119"/>
       <c r="Z88" s="119"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A89" s="119"/>
       <c r="B89" s="119"/>
       <c r="C89" s="119"/>
@@ -5074,7 +5074,7 @@
       <c r="Y89" s="119"/>
       <c r="Z89" s="119"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A90" s="119"/>
       <c r="B90" s="119"/>
       <c r="C90" s="119"/>
@@ -5102,7 +5102,7 @@
       <c r="Y90" s="119"/>
       <c r="Z90" s="119"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A91" s="119"/>
       <c r="B91" s="119"/>
       <c r="C91" s="119"/>
@@ -5130,7 +5130,7 @@
       <c r="Y91" s="119"/>
       <c r="Z91" s="119"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A92" s="119"/>
       <c r="B92" s="119"/>
       <c r="C92" s="119"/>
@@ -5158,7 +5158,7 @@
       <c r="Y92" s="119"/>
       <c r="Z92" s="119"/>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A93" s="119"/>
       <c r="B93" s="119"/>
       <c r="C93" s="119"/>
@@ -5186,7 +5186,7 @@
       <c r="Y93" s="119"/>
       <c r="Z93" s="119"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A94" s="119"/>
       <c r="B94" s="119"/>
       <c r="C94" s="119"/>
@@ -5214,7 +5214,7 @@
       <c r="Y94" s="119"/>
       <c r="Z94" s="119"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A95" s="119"/>
       <c r="B95" s="119"/>
       <c r="C95" s="119"/>
@@ -5242,7 +5242,7 @@
       <c r="Y95" s="119"/>
       <c r="Z95" s="119"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A96" s="119"/>
       <c r="B96" s="119"/>
       <c r="C96" s="119"/>
@@ -5270,7 +5270,7 @@
       <c r="Y96" s="119"/>
       <c r="Z96" s="119"/>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A97" s="119"/>
       <c r="B97" s="119"/>
       <c r="C97" s="119"/>
@@ -5298,7 +5298,7 @@
       <c r="Y97" s="119"/>
       <c r="Z97" s="119"/>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A98" s="119"/>
       <c r="B98" s="119"/>
       <c r="C98" s="119"/>
@@ -5326,7 +5326,7 @@
       <c r="Y98" s="119"/>
       <c r="Z98" s="119"/>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A99" s="119"/>
       <c r="B99" s="119"/>
       <c r="C99" s="119"/>
@@ -5383,35 +5383,35 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.86328125" customWidth="1"/>
-    <col min="2" max="2" width="15.59765625" customWidth="1"/>
-    <col min="3" max="3" width="19.3984375" customWidth="1"/>
-    <col min="4" max="4" width="14.1328125" customWidth="1"/>
-    <col min="5" max="5" width="49.1328125" customWidth="1"/>
-    <col min="6" max="6" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="49.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="12.1328125" customWidth="1"/>
-    <col min="10" max="10" width="10.1328125" customWidth="1"/>
-    <col min="11" max="11" width="7.3984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="2:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B1" s="34" t="s">
         <v>101</v>
       </c>
       <c r="C1" s="34"/>
     </row>
-    <row r="4" spans="2:10" ht="15" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B4" s="35" t="s">
         <v>102</v>
       </c>
       <c r="C4" s="35"/>
     </row>
-    <row r="6" spans="2:10" ht="17.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:10" ht="18" x14ac:dyDescent="0.25">
       <c r="B6" s="36" t="s">
         <v>103</v>
       </c>
@@ -5424,7 +5424,7 @@
       <c r="I6" s="38"/>
       <c r="J6" s="38"/>
     </row>
-    <row r="7" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="19" t="s">
         <v>82</v>
       </c>
@@ -5437,7 +5437,7 @@
       <c r="I7" s="38"/>
       <c r="J7" s="38"/>
     </row>
-    <row r="8" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="39" t="s">
         <v>83</v>
       </c>
@@ -5466,7 +5466,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="38.65" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="41" t="s">
         <v>105</v>
       </c>
@@ -5495,7 +5495,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="42" t="s">
         <v>96</v>
       </c>
@@ -5518,7 +5518,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="42"/>
       <c r="C11" s="42"/>
       <c r="D11" s="42" t="s">
@@ -5537,7 +5537,7 @@
       <c r="I11" s="42"/>
       <c r="J11" s="42"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="46" t="s">
         <v>96</v>
       </c>
@@ -5568,43 +5568,51 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B3:AE18"/>
+  <dimension ref="B2:AE18"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.86328125" customWidth="1"/>
-    <col min="2" max="2" width="15.59765625" customWidth="1"/>
-    <col min="3" max="3" width="60.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="60.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.86328125" customWidth="1"/>
-    <col min="6" max="6" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.3984375" customWidth="1"/>
-    <col min="8" max="8" width="14.3984375" customWidth="1"/>
-    <col min="9" max="9" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="12" width="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.1328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.1328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.86328125" customWidth="1"/>
-    <col min="20" max="20" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.85546875" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.86328125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.3984375" customWidth="1"/>
-    <col min="26" max="26" width="64.73046875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16.265625" customWidth="1"/>
-    <col min="30" max="30" width="16.59765625" customWidth="1"/>
-    <col min="31" max="31" width="9.265625" customWidth="1"/>
+    <col min="23" max="23" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.42578125" customWidth="1"/>
+    <col min="26" max="26" width="64.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.28515625" customWidth="1"/>
+    <col min="30" max="30" width="16.5703125" customWidth="1"/>
+    <col min="31" max="31" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="G2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="W2" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:31" x14ac:dyDescent="0.2">
       <c r="W3" s="20"/>
       <c r="X3" s="20"/>
       <c r="Y3" s="20"/>
@@ -5614,10 +5622,8 @@
       <c r="AC3" s="20"/>
       <c r="AD3" s="20"/>
     </row>
-    <row r="4" spans="2:31" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="G4" s="3" t="s">
-        <v>0</v>
-      </c>
+    <row r="4" spans="2:31" x14ac:dyDescent="0.2">
+      <c r="G4" s="3"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -5626,9 +5632,6 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="2"/>
-      <c r="W4" s="19" t="s">
-        <v>7</v>
-      </c>
       <c r="X4" s="19"/>
       <c r="Y4" s="20"/>
       <c r="Z4" s="20"/>
@@ -5638,7 +5641,7 @@
       <c r="AD4" s="20"/>
       <c r="AE4" s="20"/>
     </row>
-    <row r="5" spans="2:31" s="2" customFormat="1" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:31" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -5728,7 +5731,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:31" ht="38.65" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:31" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="50" t="s">
         <v>18</v>
       </c>
@@ -5808,7 +5811,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:31" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:31" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>28</v>
       </c>
@@ -5877,7 +5880,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="2:31" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="str">
         <f>SRV_DC_Processes!Y7</f>
         <v>S-DCE-CS-HP_N1</v>
@@ -5974,7 +5977,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9" t="s">
@@ -6006,7 +6009,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
@@ -6033,7 +6036,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -6060,7 +6063,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B12" s="32"/>
       <c r="C12" s="32"/>
       <c r="D12" s="32"/>
@@ -6087,7 +6090,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
@@ -6119,7 +6122,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B14" s="30" t="str">
         <f>SRV_DC_Processes!Y8</f>
         <v>S-DCE-CS-HE_N1</v>
@@ -6173,7 +6176,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:31" x14ac:dyDescent="0.2">
       <c r="F15" s="29">
         <v>2025</v>
       </c>
@@ -6199,7 +6202,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="2:31" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:31" x14ac:dyDescent="0.2">
       <c r="F16" s="29">
         <v>2030</v>
       </c>
@@ -6225,7 +6228,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="6:21" x14ac:dyDescent="0.35">
+    <row r="17" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F17" s="29">
         <v>2040</v>
       </c>
@@ -6251,7 +6254,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="6:21" x14ac:dyDescent="0.35">
+    <row r="18" spans="6:21" x14ac:dyDescent="0.2">
       <c r="F18" s="29">
         <v>2050</v>
       </c>
@@ -6295,23 +6298,23 @@
       <selection activeCell="P47" sqref="P47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="10.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.1328125" style="53" customWidth="1"/>
-    <col min="2" max="2" width="32.265625" style="53" customWidth="1"/>
-    <col min="3" max="7" width="6.265625" style="53" customWidth="1"/>
-    <col min="8" max="11" width="7.1328125" style="53" customWidth="1"/>
-    <col min="12" max="13" width="6.265625" style="53" customWidth="1"/>
-    <col min="14" max="16384" width="9.1328125" style="55"/>
+    <col min="1" max="1" width="2.140625" style="53" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" style="53" customWidth="1"/>
+    <col min="3" max="7" width="6.28515625" style="53" customWidth="1"/>
+    <col min="8" max="11" width="7.140625" style="53" customWidth="1"/>
+    <col min="12" max="13" width="6.28515625" style="53" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="55"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1" s="54" t="s">
         <v>248</v>
       </c>
       <c r="C1" s="54"/>
     </row>
-    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="56"/>
       <c r="B3" s="57" t="s">
         <v>44</v>
@@ -6330,7 +6333,7 @@
       <c r="L3" s="139"/>
       <c r="M3" s="140"/>
     </row>
-    <row r="4" spans="1:13" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="56"/>
       <c r="B4" s="58"/>
       <c r="C4" s="59">
@@ -6363,7 +6366,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="56"/>
       <c r="B5" s="60" t="s">
         <v>48</v>
@@ -6388,7 +6391,7 @@
       <c r="L5" s="61"/>
       <c r="M5" s="63"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="56"/>
       <c r="B6" s="64" t="s">
         <v>126</v>
@@ -6423,7 +6426,7 @@
       <c r="L6" s="68"/>
       <c r="M6" s="69"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A7" s="56"/>
       <c r="B7" s="64" t="s">
         <v>51</v>
@@ -6462,7 +6465,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A8" s="56"/>
       <c r="B8" s="73" t="s">
         <v>129</v>
@@ -6501,7 +6504,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A9" s="56"/>
       <c r="B9" s="64" t="s">
         <v>131</v>
@@ -6540,7 +6543,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="56"/>
       <c r="B10" s="64" t="s">
         <v>52</v>
@@ -6577,7 +6580,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="56"/>
       <c r="B11" s="58" t="s">
         <v>54</v>
@@ -6614,7 +6617,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="20.25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A12" s="56"/>
       <c r="B12" s="58" t="s">
         <v>56</v>
@@ -6651,7 +6654,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="56"/>
       <c r="B13" s="58" t="s">
         <v>57</v>
@@ -6690,7 +6693,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="11.65" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="56"/>
       <c r="B14" s="77" t="s">
         <v>137</v>
@@ -6727,7 +6730,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="56"/>
       <c r="B15" s="60" t="s">
         <v>59</v>
@@ -6744,7 +6747,7 @@
       <c r="L15" s="78"/>
       <c r="M15" s="63"/>
     </row>
-    <row r="16" spans="1:13" ht="20.25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A16" s="56"/>
       <c r="B16" s="58" t="s">
         <v>60</v>
@@ -6783,7 +6786,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="20.25" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A17" s="56"/>
       <c r="B17" s="58" t="s">
         <v>62</v>
@@ -6822,7 +6825,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="20.25" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A18" s="56"/>
       <c r="B18" s="58" t="s">
         <v>63</v>
@@ -6861,7 +6864,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="56"/>
       <c r="B19" s="58" t="s">
         <v>64</v>
@@ -6900,7 +6903,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="56"/>
       <c r="B20" s="58" t="s">
         <v>65</v>
@@ -6939,7 +6942,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="56"/>
       <c r="B21" s="60" t="s">
         <v>67</v>
@@ -6956,7 +6959,7 @@
       <c r="L21" s="78"/>
       <c r="M21" s="63"/>
     </row>
-    <row r="22" spans="1:13" ht="11.65" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="56"/>
       <c r="B22" s="58" t="s">
         <v>146</v>
@@ -6973,7 +6976,7 @@
       <c r="L22" s="75"/>
       <c r="M22" s="70"/>
     </row>
-    <row r="23" spans="1:13" ht="11.65" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="56"/>
       <c r="B23" s="58" t="s">
         <v>147</v>
@@ -6990,7 +6993,7 @@
       <c r="L23" s="68"/>
       <c r="M23" s="74"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="56"/>
       <c r="B24" s="58" t="s">
         <v>68</v>
@@ -7007,7 +7010,7 @@
       <c r="L24" s="68"/>
       <c r="M24" s="74"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="56"/>
       <c r="B25" s="58" t="s">
         <v>69</v>
@@ -7024,7 +7027,7 @@
       <c r="L25" s="81"/>
       <c r="M25" s="74"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="56"/>
       <c r="B26" s="58" t="s">
         <v>99</v>
@@ -7041,7 +7044,7 @@
       <c r="L26" s="81"/>
       <c r="M26" s="74"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="56"/>
       <c r="B27" s="60" t="s">
         <v>70</v>
@@ -7058,7 +7061,7 @@
       <c r="L27" s="78"/>
       <c r="M27" s="63"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="56"/>
       <c r="B28" s="58" t="s">
         <v>148</v>
@@ -7097,7 +7100,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="56"/>
       <c r="B29" s="58" t="s">
         <v>150</v>
@@ -7136,7 +7139,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="56"/>
       <c r="B30" s="58" t="s">
         <v>151</v>
@@ -7175,7 +7178,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="56"/>
       <c r="B31" s="58" t="s">
         <v>152</v>
@@ -7214,7 +7217,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="56"/>
       <c r="B32" s="58" t="s">
         <v>154</v>
@@ -7253,7 +7256,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="56"/>
       <c r="B33" s="58" t="s">
         <v>156</v>
@@ -7290,7 +7293,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="56"/>
       <c r="B34" s="83" t="s">
         <v>157</v>
@@ -7329,7 +7332,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="56"/>
       <c r="B35" s="83" t="s">
         <v>159</v>
@@ -7368,7 +7371,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="56"/>
       <c r="B36" s="58" t="s">
         <v>160</v>
@@ -7407,7 +7410,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="56"/>
       <c r="B37" s="60" t="s">
         <v>73</v>
@@ -7424,7 +7427,7 @@
       <c r="L37" s="78"/>
       <c r="M37" s="63"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="56"/>
       <c r="B38" s="58"/>
       <c r="C38" s="79"/>
@@ -7439,7 +7442,7 @@
       <c r="L38" s="68"/>
       <c r="M38" s="74"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="56"/>
       <c r="B39" s="84"/>
       <c r="C39" s="85"/>
@@ -7454,7 +7457,7 @@
       <c r="L39" s="86"/>
       <c r="M39" s="86"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="87" t="s">
         <v>162</v>
       </c>
@@ -7471,7 +7474,7 @@
       <c r="L40" s="56"/>
       <c r="M40" s="56"/>
     </row>
-    <row r="41" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="88" t="s">
         <v>97</v>
       </c>
@@ -7490,7 +7493,7 @@
       <c r="L41" s="137"/>
       <c r="M41" s="137"/>
     </row>
-    <row r="42" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="88" t="s">
         <v>164</v>
       </c>
@@ -7509,7 +7512,7 @@
       <c r="L42" s="88"/>
       <c r="M42" s="88"/>
     </row>
-    <row r="43" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="88" t="s">
         <v>98</v>
       </c>
@@ -7528,7 +7531,7 @@
       <c r="L43" s="137"/>
       <c r="M43" s="137"/>
     </row>
-    <row r="44" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="88" t="s">
         <v>58</v>
       </c>
@@ -7547,7 +7550,7 @@
       <c r="L44" s="137"/>
       <c r="M44" s="137"/>
     </row>
-    <row r="45" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="88" t="s">
         <v>61</v>
       </c>
@@ -7566,7 +7569,7 @@
       <c r="L45" s="137"/>
       <c r="M45" s="137"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="88" t="s">
         <v>66</v>
       </c>
@@ -7585,7 +7588,7 @@
       <c r="L46" s="89"/>
       <c r="M46" s="89"/>
     </row>
-    <row r="47" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="88" t="s">
         <v>72</v>
       </c>
@@ -7604,7 +7607,7 @@
       <c r="L47" s="137"/>
       <c r="M47" s="137"/>
     </row>
-    <row r="48" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="88" t="s">
         <v>53</v>
       </c>
@@ -7623,7 +7626,7 @@
       <c r="L48" s="137"/>
       <c r="M48" s="137"/>
     </row>
-    <row r="49" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="88" t="s">
         <v>55</v>
       </c>
@@ -7642,7 +7645,7 @@
       <c r="L49" s="137"/>
       <c r="M49" s="137"/>
     </row>
-    <row r="50" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="88" t="s">
         <v>173</v>
       </c>
@@ -7661,7 +7664,7 @@
       <c r="L50" s="137"/>
       <c r="M50" s="137"/>
     </row>
-    <row r="51" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="88" t="s">
         <v>153</v>
       </c>
@@ -7680,7 +7683,7 @@
       <c r="L51" s="137"/>
       <c r="M51" s="137"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="88" t="s">
         <v>176</v>
       </c>
@@ -7699,7 +7702,7 @@
       <c r="L52" s="90"/>
       <c r="M52" s="90"/>
     </row>
-    <row r="53" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="88" t="s">
         <v>155</v>
       </c>
@@ -7718,7 +7721,7 @@
       <c r="L53" s="137"/>
       <c r="M53" s="137"/>
     </row>
-    <row r="54" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="88" t="s">
         <v>71</v>
       </c>
@@ -7737,7 +7740,7 @@
       <c r="L54" s="137"/>
       <c r="M54" s="137"/>
     </row>
-    <row r="55" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="88" t="s">
         <v>161</v>
       </c>
@@ -7756,7 +7759,7 @@
       <c r="L55" s="137"/>
       <c r="M55" s="137"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="56" t="s">
         <v>181</v>
       </c>
@@ -7764,7 +7767,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="87"/>
       <c r="B57" s="56"/>
       <c r="C57" s="91"/>
@@ -7779,7 +7782,7 @@
       <c r="L57" s="91"/>
       <c r="M57" s="91"/>
     </row>
-    <row r="58" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="87" t="s">
         <v>183</v>
       </c>
@@ -7796,7 +7799,7 @@
       <c r="L58" s="92"/>
       <c r="M58" s="92"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="92">
         <v>1</v>
       </c>
@@ -7815,7 +7818,7 @@
       <c r="L59" s="92"/>
       <c r="M59" s="92"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="92">
         <v>2</v>
       </c>
@@ -7834,7 +7837,7 @@
       <c r="L60" s="92"/>
       <c r="M60" s="92"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="92">
         <v>3</v>
       </c>
@@ -7853,7 +7856,7 @@
       <c r="L61" s="94"/>
       <c r="M61" s="94"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" s="92">
         <v>4</v>
       </c>
@@ -7872,7 +7875,7 @@
       <c r="L62" s="94"/>
       <c r="M62" s="94"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" s="92">
         <v>5</v>
       </c>
@@ -7891,7 +7894,7 @@
       <c r="L63" s="94"/>
       <c r="M63" s="94"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" s="92">
         <v>6</v>
       </c>
@@ -7910,7 +7913,7 @@
       <c r="L64" s="84"/>
       <c r="M64" s="84"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" s="92">
         <v>7</v>
       </c>
@@ -7929,7 +7932,7 @@
       <c r="L65" s="84"/>
       <c r="M65" s="84"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" s="92">
         <v>8</v>
       </c>
@@ -7948,7 +7951,7 @@
       <c r="L66" s="84"/>
       <c r="M66" s="84"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" s="92">
         <v>9</v>
       </c>
@@ -7967,7 +7970,7 @@
       <c r="L67" s="84"/>
       <c r="M67" s="84"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A68" s="92">
         <v>10</v>
       </c>
@@ -7986,7 +7989,7 @@
       <c r="L68" s="84"/>
       <c r="M68" s="84"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" s="92">
         <v>11</v>
       </c>
@@ -7994,7 +7997,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" s="92">
         <v>12</v>
       </c>
@@ -8002,7 +8005,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" s="92">
         <v>13</v>
       </c>
@@ -8010,7 +8013,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" s="92">
         <v>14</v>
       </c>
@@ -8018,7 +8021,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" s="92">
         <v>15</v>
       </c>
@@ -8026,7 +8029,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" s="92">
         <v>16</v>
       </c>
@@ -8034,7 +8037,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" s="92">
         <v>17</v>
       </c>
@@ -8042,7 +8045,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" s="92">
         <v>18</v>
       </c>
@@ -8050,7 +8053,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="83" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B83" s="96"/>
       <c r="C83" s="97"/>
       <c r="D83" s="97"/>
@@ -8064,11 +8067,11 @@
       <c r="L83" s="97"/>
       <c r="M83" s="97"/>
     </row>
-    <row r="86" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C86" s="98"/>
       <c r="D86" s="98"/>
     </row>
-    <row r="87" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C87" s="99"/>
       <c r="D87" s="99"/>
       <c r="E87" s="99"/>
@@ -8076,6 +8079,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B44:M44"/>
+    <mergeCell ref="C3:M3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="B41:M41"/>
+    <mergeCell ref="B43:M43"/>
     <mergeCell ref="B53:M53"/>
     <mergeCell ref="B54:M54"/>
     <mergeCell ref="B55:M55"/>
@@ -8085,12 +8094,6 @@
     <mergeCell ref="B49:M49"/>
     <mergeCell ref="B50:M50"/>
     <mergeCell ref="B51:M51"/>
-    <mergeCell ref="B44:M44"/>
-    <mergeCell ref="C3:M3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="B41:M41"/>
-    <mergeCell ref="B43:M43"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C3" location="INDEX" display="Heat pumps utilizing industrial waste heat 3 MW" xr:uid="{42BCD51D-8F42-4398-853E-66F8A7B17C5C}"/>
@@ -8111,20 +8114,20 @@
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="10.15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.59765625" style="100" customWidth="1"/>
-    <col min="2" max="2" width="43.3984375" style="100" customWidth="1"/>
-    <col min="3" max="13" width="10.1328125" style="100" customWidth="1"/>
-    <col min="14" max="16384" width="9.1328125" style="100"/>
+    <col min="1" max="1" width="3.5703125" style="100" customWidth="1"/>
+    <col min="2" max="2" width="43.42578125" style="100" customWidth="1"/>
+    <col min="3" max="13" width="10.140625" style="100" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="100"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1" s="54" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="11.65" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="12" x14ac:dyDescent="0.2">
       <c r="A3" s="143" t="s">
         <v>44</v>
       </c>
@@ -8143,7 +8146,7 @@
       <c r="L3" s="145"/>
       <c r="M3" s="145"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="146" t="s">
         <v>208</v>
       </c>
@@ -8182,7 +8185,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="147" t="s">
         <v>209</v>
       </c>
@@ -8221,7 +8224,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="103" t="s">
         <v>215</v>
       </c>
@@ -8240,7 +8243,7 @@
       <c r="L6" s="101"/>
       <c r="M6" s="101"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="104" t="s">
         <v>48</v>
       </c>
@@ -8257,7 +8260,7 @@
       <c r="L7" s="105"/>
       <c r="M7" s="105"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="105"/>
       <c r="B8" s="106" t="s">
         <v>249</v>
@@ -8294,7 +8297,7 @@
       </c>
       <c r="M8" s="107"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="105"/>
       <c r="B9" s="106" t="s">
         <v>250</v>
@@ -8329,7 +8332,7 @@
       <c r="L9" s="107"/>
       <c r="M9" s="107"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="105"/>
       <c r="B10" s="106" t="s">
         <v>251</v>
@@ -8364,7 +8367,7 @@
       <c r="L10" s="107"/>
       <c r="M10" s="107"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="105"/>
       <c r="B11" s="106" t="s">
         <v>252</v>
@@ -8401,7 +8404,7 @@
       </c>
       <c r="M11" s="107"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="105"/>
       <c r="B12" s="106" t="s">
         <v>253</v>
@@ -8438,7 +8441,7 @@
       </c>
       <c r="M12" s="107"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B13" s="106" t="s">
         <v>254</v>
       </c>
@@ -8474,7 +8477,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="104" t="s">
         <v>219</v>
       </c>
@@ -8491,7 +8494,7 @@
       <c r="L14" s="110"/>
       <c r="M14" s="110"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="105"/>
       <c r="B15" s="106" t="s">
         <v>255</v>
@@ -8508,7 +8511,7 @@
       <c r="L15" s="107"/>
       <c r="M15" s="107"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="105"/>
       <c r="B16" s="106" t="s">
         <v>256</v>
@@ -8525,7 +8528,7 @@
       <c r="L16" s="107"/>
       <c r="M16" s="107"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="105"/>
       <c r="B17" s="106" t="s">
         <v>257</v>
@@ -8542,7 +8545,7 @@
       <c r="L17" s="107"/>
       <c r="M17" s="107"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="105"/>
       <c r="B18" s="106" t="s">
         <v>258</v>
@@ -8559,7 +8562,7 @@
       <c r="L18" s="107"/>
       <c r="M18" s="107"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="105"/>
       <c r="B19" s="106" t="s">
         <v>259</v>
@@ -8576,7 +8579,7 @@
       <c r="L19" s="107"/>
       <c r="M19" s="107"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="104" t="s">
         <v>67</v>
       </c>
@@ -8593,7 +8596,7 @@
       <c r="L20" s="110"/>
       <c r="M20" s="110"/>
     </row>
-    <row r="21" spans="1:13" ht="11.65" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="105"/>
       <c r="B21" s="106" t="s">
         <v>220</v>
@@ -8610,7 +8613,7 @@
       <c r="L21" s="107"/>
       <c r="M21" s="107"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="105"/>
       <c r="B22" s="111" t="s">
         <v>221</v>
@@ -8627,7 +8630,7 @@
       <c r="L22" s="107"/>
       <c r="M22" s="107"/>
     </row>
-    <row r="23" spans="1:13" ht="11.65" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="105"/>
       <c r="B23" s="111" t="s">
         <v>222</v>
@@ -8644,7 +8647,7 @@
       <c r="L23" s="107"/>
       <c r="M23" s="107"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="105"/>
       <c r="B24" s="111" t="s">
         <v>223</v>
@@ -8661,7 +8664,7 @@
       <c r="L24" s="107"/>
       <c r="M24" s="107"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="105"/>
       <c r="B25" s="111" t="s">
         <v>224</v>
@@ -8678,7 +8681,7 @@
       <c r="L25" s="107"/>
       <c r="M25" s="107"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="104" t="s">
         <v>100</v>
       </c>
@@ -8695,7 +8698,7 @@
       <c r="L26" s="110"/>
       <c r="M26" s="110"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B27" s="111" t="s">
         <v>225</v>
       </c>
@@ -8733,7 +8736,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B28" s="111" t="s">
         <v>227</v>
       </c>
@@ -8767,7 +8770,7 @@
       <c r="L28" s="108"/>
       <c r="M28" s="108"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B29" s="111" t="s">
         <v>228</v>
       </c>
@@ -8801,7 +8804,7 @@
       <c r="L29" s="108"/>
       <c r="M29" s="108"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B30" s="111" t="s">
         <v>229</v>
       </c>
@@ -8837,7 +8840,7 @@
       </c>
       <c r="M30" s="108"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="105"/>
       <c r="B31" s="106" t="s">
         <v>260</v>
@@ -8874,7 +8877,7 @@
       </c>
       <c r="M31" s="107"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B32" s="106" t="s">
         <v>261</v>
       </c>
@@ -8908,7 +8911,7 @@
       <c r="L32" s="108"/>
       <c r="M32" s="108"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B33" s="106" t="s">
         <v>262</v>
       </c>
@@ -8942,7 +8945,7 @@
       <c r="L33" s="108"/>
       <c r="M33" s="108"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="105"/>
       <c r="B34" s="106" t="s">
         <v>263</v>
@@ -8977,7 +8980,7 @@
       <c r="L34" s="107"/>
       <c r="M34" s="107"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="116" t="s">
         <v>73</v>
       </c>
@@ -8994,7 +8997,7 @@
       <c r="L35" s="110"/>
       <c r="M35" s="110"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="116"/>
       <c r="B36" s="116"/>
       <c r="C36" s="109"/>
@@ -9009,7 +9012,7 @@
       <c r="L36" s="110"/>
       <c r="M36" s="110"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="116"/>
       <c r="B37" s="116"/>
       <c r="C37" s="109"/>
@@ -9024,100 +9027,100 @@
       <c r="L37" s="110"/>
       <c r="M37" s="110"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="117" t="s">
         <v>231</v>
       </c>
       <c r="L38" s="108"/>
       <c r="M38" s="108"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="108"/>
       <c r="B39" s="100" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="108"/>
       <c r="B40" s="100" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="108"/>
       <c r="B41" s="100" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="108"/>
       <c r="B42" s="100" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="108"/>
       <c r="B43" s="100" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="108"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="117" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="108"/>
       <c r="B46" s="100" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="108"/>
       <c r="B47" s="100" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="108"/>
       <c r="B48" s="100" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="108"/>
       <c r="B49" s="100" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="108"/>
       <c r="B50" s="100" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="108"/>
       <c r="B51" s="100" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="108"/>
       <c r="B52" s="100" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="108"/>
       <c r="B53" s="100" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="108"/>
       <c r="B54" s="100" t="s">
         <v>246</v>

</xml_diff>

<commit_message>
Fix Data C DH
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_SRV_DC_ExcessHeat.xlsx
+++ b/SubRES_TMPL/SubRES_SRV_DC_ExcessHeat.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A48014D-F089-40DF-9FDA-681C19B19723}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FAF3CCF-417F-4082-87FD-8BC3CDF3A799}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="16" r:id="rId1"/>
@@ -5379,7 +5379,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:J12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -5570,8 +5570,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:AE18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5579,7 +5579,7 @@
     <col min="1" max="1" width="5.85546875" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
     <col min="3" max="3" width="60.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" customWidth="1"/>
@@ -8079,12 +8079,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B44:M44"/>
-    <mergeCell ref="C3:M3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="B41:M41"/>
-    <mergeCell ref="B43:M43"/>
     <mergeCell ref="B53:M53"/>
     <mergeCell ref="B54:M54"/>
     <mergeCell ref="B55:M55"/>
@@ -8094,6 +8088,12 @@
     <mergeCell ref="B49:M49"/>
     <mergeCell ref="B50:M50"/>
     <mergeCell ref="B51:M51"/>
+    <mergeCell ref="B44:M44"/>
+    <mergeCell ref="C3:M3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="B41:M41"/>
+    <mergeCell ref="B43:M43"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C3" location="INDEX" display="Heat pumps utilizing industrial waste heat 3 MW" xr:uid="{42BCD51D-8F42-4398-853E-66F8A7B17C5C}"/>

</xml_diff>